<commit_message>
subfinder is working without api keys atm.
</commit_message>
<xml_diff>
--- a/osint_report.xlsx
+++ b/osint_report.xlsx
@@ -2,29 +2,32 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="34785" yWindow="1515" windowWidth="28605" windowHeight="19365" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Employees" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Emails" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Subfinder" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -38,12 +41,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -56,14 +74,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -426,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,447 +456,163 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Datetime</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Search</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Title</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>URL</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>rawText</t>
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Subdomains</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>bing</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>laurie j. o'hara</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Vice President &amp; Corporate Secretary</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/laurie-j-o-hara-99101a68</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Laurie J. O'Hara - Vice President &amp; Corporate Secretary - LinkedIn</t>
+          <t>www.dceres.unitedradio.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>bing</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>brian dumond</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>President</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/brian-dumond-9618591b</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Brian DuMond - President - Geddes Federal Savings and Loan Association ...</t>
+          <t>www.mysqlclone.unitedradio.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>bing</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>chris lauricella nmls#491199</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Assistant Vice President</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/chris-lauricella-nmls-491199-637b432b</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Chris Lauricella NMLS#491199 - Assistant Vice President</t>
+          <t>auto-rtr.unitedradio.com</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>bing</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>johanna dorrance</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Vice President</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/johanna-dorrance-7524482a</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Johanna Dorrance - Vice President - Geddes Federal Savings</t>
+          <t>sony.unitedradio.com</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>bing</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>melissa daniels</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Electronic Banking Service Manager/Assistant</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/melissa-daniels-a9a98112</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Melissa Daniels - Electronic Banking Service Manager/Assistant </t>
+          <t>www.vpn2.unitedradio.com</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>bing</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>betsy bernardin</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Assistant Secretary</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/betsy-bernardin-468a386a</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Betsy Bernardin - Assistant Secretary - LinkedIn</t>
+          <t>eres.unitedradio.com</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>bing</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>geddes federal savings and loan association</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>LinkedIn</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/linda-pendock-239a4068</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Geddes Federal Savings and Loan Association - LinkedIn</t>
+          <t>dceresdev.unitedradio.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>bing</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>geddes federal savings and loan association</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>LinkedIn</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/sarah-munnell-a01261189</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Geddes Federal Savings and Loan Association - LinkedIn</t>
+          <t>dealerconnect.unitedradio.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>bing</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>karen henderson</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Flaig</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/karen-henderson-flaig-49481666</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Karen Henderson-Flaig - Customer Service Representative</t>
+          <t>dceres.unitedradio.com</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bing</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>patti orioli nmls #491200</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Assistant Vice President/ Loan</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/patti-orioli-nmls-491200-4b991290</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Patti Orioli NMLS #491200 - Assistant Vice President/ Loan</t>
+          <t>vpn2.unitedradio.com</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>bing</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>brian dumond</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>President</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/brian-dumond-9618591b</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Brian DuMond - President - Geddes Federal Savings and Loan Association </t>
+          <t>ws.unitedradio.com</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>bing</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>chris lauricella nmls#491199</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Assistant Vice President</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>https://www.linkedin.com/in/chris-lauricella-nmls-491199-637b432b</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Chris Lauricella NMLS#491199 - Assistant Vice President - LinkedIn</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Emails</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>l.o'hara@geddesfederal.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>b.dumond@geddesfederal.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>c.nmls#491199@geddesfederal.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>j.dorrance@geddesfederal.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>m.daniels@geddesfederal.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>b.bernardin@geddesfederal.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>g.association@geddesfederal.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>k.henderson@geddesfederal.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>p.#491200@geddesfederal.com</t>
+          <t>mysqlclone.unitedradio.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>vpn1.unitedradio.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>mysqlclone-new.unitedradio.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>www.web2.unitedradio.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>www.vpn1.unitedradio.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>wa.unitedradio.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>www.unitedradio.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>web.unitedradio.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>mail.unitedradio.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>web2.unitedradio.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>www.ws.unitedradio.com</t>
         </is>
       </c>
     </row>

</xml_diff>